<commit_message>
working fine but not detecting some bikes
</commit_message>
<xml_diff>
--- a/traffic_segments.xlsx
+++ b/traffic_segments.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Segment_1_0_60" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Segment_1_0_120" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E82"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +465,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -474,11 +474,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.02</v>
+        <v>4.36</v>
       </c>
     </row>
     <row r="3">
@@ -486,11 +486,11 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.38</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="4">
@@ -507,7 +507,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -516,11 +516,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>1.8</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -528,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -537,11 +537,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2.34</v>
+        <v>9.32</v>
       </c>
     </row>
     <row r="6">
@@ -549,7 +549,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -558,11 +558,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>4.6</v>
+        <v>9.68</v>
       </c>
     </row>
     <row r="7">
@@ -570,7 +570,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -579,11 +579,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>4.82</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="8">
@@ -591,11 +591,11 @@
         <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -604,7 +604,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>5.14</v>
+        <v>14.74</v>
       </c>
     </row>
     <row r="9">
@@ -612,7 +612,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -621,11 +621,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>5.16</v>
+        <v>15.44</v>
       </c>
     </row>
     <row r="10">
@@ -633,20 +633,20 @@
         <v>1</v>
       </c>
       <c r="B10" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>8.9</v>
+        <v>15.84</v>
       </c>
     </row>
     <row r="11">
@@ -654,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -663,11 +663,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>9.6</v>
+        <v>18.72</v>
       </c>
     </row>
     <row r="12">
@@ -675,11 +675,11 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>9.960000000000001</v>
+        <v>20.42</v>
       </c>
     </row>
     <row r="13">
@@ -696,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -705,11 +705,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>14.48</v>
+        <v>20.62</v>
       </c>
     </row>
     <row r="14">
@@ -717,11 +717,11 @@
         <v>1</v>
       </c>
       <c r="B14" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>14.78</v>
+        <v>20.82</v>
       </c>
     </row>
     <row r="15">
@@ -738,11 +738,11 @@
         <v>1</v>
       </c>
       <c r="B15" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>14.84</v>
+        <v>21.18</v>
       </c>
     </row>
     <row r="16">
@@ -759,20 +759,20 @@
         <v>1</v>
       </c>
       <c r="B16" t="n">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>15.06</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="17">
@@ -780,11 +780,11 @@
         <v>1</v>
       </c>
       <c r="B17" t="n">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>15.78</v>
+        <v>22.9</v>
       </c>
     </row>
     <row r="18">
@@ -801,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="n">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -814,7 +814,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>16.82</v>
+        <v>23.36</v>
       </c>
     </row>
     <row r="19">
@@ -822,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>17.48</v>
+        <v>24.68</v>
       </c>
     </row>
     <row r="20">
@@ -843,7 +843,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -856,7 +856,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>18.28</v>
+        <v>25.04</v>
       </c>
     </row>
     <row r="21">
@@ -864,11 +864,11 @@
         <v>1</v>
       </c>
       <c r="B21" t="n">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -877,7 +877,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>19.16</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="22">
@@ -885,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -894,11 +894,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>20.28</v>
+        <v>28.64</v>
       </c>
     </row>
     <row r="23">
@@ -906,11 +906,11 @@
         <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -919,7 +919,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>20.88</v>
+        <v>28.96</v>
       </c>
     </row>
     <row r="24">
@@ -927,11 +927,11 @@
         <v>1</v>
       </c>
       <c r="B24" t="n">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>21.5</v>
+        <v>30.86</v>
       </c>
     </row>
     <row r="25">
@@ -948,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="n">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -957,11 +957,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>22.74</v>
+        <v>30.98</v>
       </c>
     </row>
     <row r="26">
@@ -969,11 +969,11 @@
         <v>1</v>
       </c>
       <c r="B26" t="n">
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>23.04</v>
+        <v>35.7</v>
       </c>
     </row>
     <row r="27">
@@ -990,11 +990,11 @@
         <v>1</v>
       </c>
       <c r="B27" t="n">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>truck</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1003,7 +1003,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>23.18</v>
+        <v>36.3</v>
       </c>
     </row>
     <row r="28">
@@ -1011,7 +1011,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="n">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>24.78</v>
+        <v>36.62</v>
       </c>
     </row>
     <row r="29">
@@ -1032,20 +1032,20 @@
         <v>1</v>
       </c>
       <c r="B29" t="n">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>24.96</v>
+        <v>38.94</v>
       </c>
     </row>
     <row r="30">
@@ -1053,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="n">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1066,7 +1066,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>26.42</v>
+        <v>41.34</v>
       </c>
     </row>
     <row r="31">
@@ -1074,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="B31" t="n">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1083,11 +1083,11 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>27.96</v>
+        <v>42.86</v>
       </c>
     </row>
     <row r="32">
@@ -1095,20 +1095,20 @@
         <v>1</v>
       </c>
       <c r="B32" t="n">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>29</v>
+        <v>43.42</v>
       </c>
     </row>
     <row r="33">
@@ -1116,20 +1116,20 @@
         <v>1</v>
       </c>
       <c r="B33" t="n">
-        <v>80</v>
+        <v>21</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>29.76</v>
+        <v>44.92</v>
       </c>
     </row>
     <row r="34">
@@ -1137,20 +1137,20 @@
         <v>1</v>
       </c>
       <c r="B34" t="n">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>29.96</v>
+        <v>46.86</v>
       </c>
     </row>
     <row r="35">
@@ -1158,20 +1158,20 @@
         <v>1</v>
       </c>
       <c r="B35" t="n">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>30.6</v>
+        <v>47.34</v>
       </c>
     </row>
     <row r="36">
@@ -1179,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="B36" t="n">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>31.32</v>
+        <v>49.88</v>
       </c>
     </row>
     <row r="37">
@@ -1200,20 +1200,20 @@
         <v>1</v>
       </c>
       <c r="B37" t="n">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>33.34</v>
+        <v>53.24</v>
       </c>
     </row>
     <row r="38">
@@ -1221,7 +1221,7 @@
         <v>1</v>
       </c>
       <c r="B38" t="n">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1234,7 +1234,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>35.3</v>
+        <v>53.56</v>
       </c>
     </row>
     <row r="39">
@@ -1242,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="B39" t="n">
-        <v>103</v>
+        <v>28</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1251,11 +1251,11 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>35.48</v>
+        <v>56.08</v>
       </c>
     </row>
     <row r="40">
@@ -1263,20 +1263,20 @@
         <v>1</v>
       </c>
       <c r="B40" t="n">
-        <v>107</v>
+        <v>28</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>36.08</v>
+        <v>56.56</v>
       </c>
     </row>
     <row r="41">
@@ -1284,7 +1284,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="n">
-        <v>111</v>
+        <v>29</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -1297,7 +1297,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>36.38</v>
+        <v>59.82</v>
       </c>
     </row>
     <row r="42">
@@ -1305,7 +1305,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="n">
-        <v>113</v>
+        <v>31</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -1314,11 +1314,11 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>36.7</v>
+        <v>62.32</v>
       </c>
     </row>
     <row r="43">
@@ -1326,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="n">
-        <v>112</v>
+        <v>18</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>37.2</v>
+        <v>67.22</v>
       </c>
     </row>
     <row r="44">
@@ -1347,7 +1347,7 @@
         <v>1</v>
       </c>
       <c r="B44" t="n">
-        <v>127</v>
+        <v>27</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1356,11 +1356,11 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>37.98</v>
+        <v>71.18000000000001</v>
       </c>
     </row>
     <row r="45">
@@ -1368,20 +1368,20 @@
         <v>1</v>
       </c>
       <c r="B45" t="n">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>truck</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>38.28</v>
+        <v>78.14</v>
       </c>
     </row>
     <row r="46">
@@ -1389,7 +1389,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="n">
-        <v>123</v>
+        <v>36</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>38.46</v>
+        <v>78.58</v>
       </c>
     </row>
     <row r="47">
@@ -1410,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="B47" t="n">
-        <v>131</v>
+        <v>36</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -1419,11 +1419,11 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>38.56</v>
+        <v>79.08</v>
       </c>
     </row>
     <row r="48">
@@ -1431,11 +1431,11 @@
         <v>1</v>
       </c>
       <c r="B48" t="n">
-        <v>140</v>
+        <v>14</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1444,7 +1444,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>39.4</v>
+        <v>79.09999999999999</v>
       </c>
     </row>
     <row r="49">
@@ -1452,20 +1452,20 @@
         <v>1</v>
       </c>
       <c r="B49" t="n">
-        <v>142</v>
+        <v>37</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>39.62</v>
+        <v>79.92</v>
       </c>
     </row>
     <row r="50">
@@ -1473,11 +1473,11 @@
         <v>1</v>
       </c>
       <c r="B50" t="n">
-        <v>138</v>
+        <v>37</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1486,7 +1486,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>39.62</v>
+        <v>80.54000000000001</v>
       </c>
     </row>
     <row r="51">
@@ -1494,7 +1494,7 @@
         <v>1</v>
       </c>
       <c r="B51" t="n">
-        <v>119</v>
+        <v>30</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -1503,11 +1503,11 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>39.62</v>
+        <v>84.81999999999999</v>
       </c>
     </row>
     <row r="52">
@@ -1515,7 +1515,7 @@
         <v>1</v>
       </c>
       <c r="B52" t="n">
-        <v>137</v>
+        <v>32</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -1528,7 +1528,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>39.7</v>
+        <v>90.38</v>
       </c>
     </row>
     <row r="53">
@@ -1536,7 +1536,7 @@
         <v>1</v>
       </c>
       <c r="B53" t="n">
-        <v>145</v>
+        <v>29</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -1545,11 +1545,11 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>40.06</v>
+        <v>90.76000000000001</v>
       </c>
     </row>
     <row r="54">
@@ -1557,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="B54" t="n">
-        <v>147</v>
+        <v>40</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1570,7 +1570,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>40.84</v>
+        <v>91.09999999999999</v>
       </c>
     </row>
     <row r="55">
@@ -1578,20 +1578,20 @@
         <v>1</v>
       </c>
       <c r="B55" t="n">
-        <v>148</v>
+        <v>40</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>41.12</v>
+        <v>91.09999999999999</v>
       </c>
     </row>
     <row r="56">
@@ -1599,7 +1599,7 @@
         <v>1</v>
       </c>
       <c r="B56" t="n">
-        <v>157</v>
+        <v>39</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1608,11 +1608,11 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>41.62</v>
+        <v>92.28</v>
       </c>
     </row>
     <row r="57">
@@ -1620,7 +1620,7 @@
         <v>1</v>
       </c>
       <c r="B57" t="n">
-        <v>160</v>
+        <v>16</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -1629,11 +1629,11 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>41.74</v>
+        <v>96.88</v>
       </c>
     </row>
     <row r="58">
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="B58" t="n">
-        <v>158</v>
+        <v>41</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -1650,11 +1650,11 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>42.26</v>
+        <v>97.18000000000001</v>
       </c>
     </row>
     <row r="59">
@@ -1662,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="B59" t="n">
-        <v>166</v>
+        <v>42</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -1675,7 +1675,7 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>43.12</v>
+        <v>98.08</v>
       </c>
     </row>
     <row r="60">
@@ -1683,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="B60" t="n">
-        <v>165</v>
+        <v>42</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -1692,11 +1692,11 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>43.32</v>
+        <v>98.59999999999999</v>
       </c>
     </row>
     <row r="61">
@@ -1704,7 +1704,7 @@
         <v>1</v>
       </c>
       <c r="B61" t="n">
-        <v>170</v>
+        <v>44</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -1713,11 +1713,11 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>43.78</v>
+        <v>100.44</v>
       </c>
     </row>
     <row r="62">
@@ -1725,7 +1725,7 @@
         <v>1</v>
       </c>
       <c r="B62" t="n">
-        <v>171</v>
+        <v>43</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1734,11 +1734,11 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>43.8</v>
+        <v>103.04</v>
       </c>
     </row>
     <row r="63">
@@ -1746,20 +1746,20 @@
         <v>1</v>
       </c>
       <c r="B63" t="n">
-        <v>173</v>
+        <v>45</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>44.7</v>
+        <v>109.72</v>
       </c>
     </row>
     <row r="64">
@@ -1767,20 +1767,20 @@
         <v>1</v>
       </c>
       <c r="B64" t="n">
-        <v>178</v>
+        <v>45</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Down</t>
+          <t>Up</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>45.18</v>
+        <v>110.18</v>
       </c>
     </row>
     <row r="65">
@@ -1788,20 +1788,20 @@
         <v>1</v>
       </c>
       <c r="B65" t="n">
-        <v>183</v>
+        <v>46</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>motorbike</t>
+          <t>car</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Up</t>
+          <t>Down</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>46.46</v>
+        <v>112.6</v>
       </c>
     </row>
     <row r="66">
@@ -1809,7 +1809,7 @@
         <v>1</v>
       </c>
       <c r="B66" t="n">
-        <v>167</v>
+        <v>46</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>47.12</v>
+        <v>112.98</v>
       </c>
     </row>
     <row r="67">
@@ -1830,11 +1830,11 @@
         <v>1</v>
       </c>
       <c r="B67" t="n">
-        <v>182</v>
+        <v>33</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>car</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1843,7 +1843,7 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>47.2</v>
+        <v>116.46</v>
       </c>
     </row>
     <row r="68">
@@ -1851,11 +1851,11 @@
         <v>1</v>
       </c>
       <c r="B68" t="n">
-        <v>189</v>
+        <v>49</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>truck</t>
+          <t>motorbike</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1864,301 +1864,7 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>47.5</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>1</v>
-      </c>
-      <c r="B69" t="n">
-        <v>169</v>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>car</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="E69" t="n">
-        <v>48.26</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>1</v>
-      </c>
-      <c r="B70" t="n">
-        <v>184</v>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>car</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="E70" t="n">
-        <v>48.48</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>1</v>
-      </c>
-      <c r="B71" t="n">
-        <v>187</v>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>car</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="E71" t="n">
-        <v>50.16</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>1</v>
-      </c>
-      <c r="B72" t="n">
-        <v>198</v>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>motorbike</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>Down</t>
-        </is>
-      </c>
-      <c r="E72" t="n">
-        <v>50.18</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>1</v>
-      </c>
-      <c r="B73" t="n">
-        <v>188</v>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>car</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="E73" t="n">
-        <v>52.16</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>1</v>
-      </c>
-      <c r="B74" t="n">
-        <v>205</v>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>motorbike</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="E74" t="n">
-        <v>53.04</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>1</v>
-      </c>
-      <c r="B75" t="n">
-        <v>202</v>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>car</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="E75" t="n">
-        <v>53.2</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>1</v>
-      </c>
-      <c r="B76" t="n">
-        <v>208</v>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>motorbike</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>Down</t>
-        </is>
-      </c>
-      <c r="E76" t="n">
-        <v>53.46</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n">
-        <v>1</v>
-      </c>
-      <c r="B77" t="n">
-        <v>212</v>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>motorbike</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>Down</t>
-        </is>
-      </c>
-      <c r="E77" t="n">
-        <v>53.96</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="n">
-        <v>1</v>
-      </c>
-      <c r="B78" t="n">
-        <v>213</v>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>motorbike</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>Down</t>
-        </is>
-      </c>
-      <c r="E78" t="n">
-        <v>54.68</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n">
-        <v>1</v>
-      </c>
-      <c r="B79" t="n">
-        <v>192</v>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>car</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="E79" t="n">
-        <v>54.98</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="n">
-        <v>1</v>
-      </c>
-      <c r="B80" t="n">
-        <v>217</v>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>car</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>Down</t>
-        </is>
-      </c>
-      <c r="E80" t="n">
-        <v>56.44</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n">
-        <v>1</v>
-      </c>
-      <c r="B81" t="n">
-        <v>223</v>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>motorbike</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="E81" t="n">
-        <v>58.1</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n">
-        <v>1</v>
-      </c>
-      <c r="B82" t="n">
-        <v>227</v>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>motorbike</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="E82" t="n">
-        <v>59.18</v>
+        <v>117.84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>